<commit_message>
working on ion mass exclusion
</commit_message>
<xml_diff>
--- a/Data/Data_Citations.xlsx
+++ b/Data/Data_Citations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\linne\Box Sync\CL_BUD\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78067BBF-0549-4297-A24C-E30B73F61714}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A28F9FD2-E3D4-42B6-AAC0-4D3F424AB59E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="768" yWindow="768" windowWidth="17280" windowHeight="8964" xr2:uid="{02D620E8-8DA4-42D6-925F-9D866E7AA299}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{02D620E8-8DA4-42D6-925F-9D866E7AA299}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="54">
   <si>
     <t xml:space="preserve">Dataset Title </t>
   </si>
@@ -276,14 +276,41 @@
     <t>?? How to cite USGS data? I also need to cite the sp. conductivity to USGS</t>
   </si>
   <si>
-    <t xml:space="preserve">barometric pressure </t>
-  </si>
-  <si>
     <t>AOS barometric pressure data for water level calculation</t>
   </si>
   <si>
     <t>Space Science &amp; Engineering Center UW-Madison
 how do I cite this??</t>
+  </si>
+  <si>
+    <t>Robertson, D., J. Magnuson, S. Carpenter, and E. Stanley. 2014. North Temperate Lakes LTER Morphometry and Hypsometry data for core study lakes ver 1. Environmental Data Initiative. https://doi.org/10.6073/pasta/1d15f38aaf14110714add6230ef78bd8. Accessed 2020-06-23.</t>
+  </si>
+  <si>
+    <t>Hypsometry data for ME and MO</t>
+  </si>
+  <si>
+    <t>lake_hypsometry</t>
+  </si>
+  <si>
+    <t>level_data.rds</t>
+  </si>
+  <si>
+    <t>N. Lead PI, J. Magnuson, S. Carpenter, and E. Stanley. 2020. North Temperate Lakes LTER: Snow and Ice Depth 1982 - current ver 31. Environmental Data Initiative. https://doi.org/10.6073/pasta/f4e281545ec5c5c18dc996cf652f5f8c. Accessed 2020-06-23.</t>
+  </si>
+  <si>
+    <t>ice thickness ME and MO</t>
+  </si>
+  <si>
+    <t>winter</t>
+  </si>
+  <si>
+    <t>N. Lead PI, N. LTER, J. Magnuson, S. Carpenter, and E. Stanley. 2020. North Temperate Lakes LTER: Ice Duration - Madison Lakes Area 1853 - current ver 34. Environmental Data Initiative. https://doi.org/10.6073/pasta/22a5b5f8bce193353e559918b0024f9d. Accessed 2020-06-23.</t>
+  </si>
+  <si>
+    <t>ice on off dates ME and MO</t>
+  </si>
+  <si>
+    <t>icedates</t>
   </si>
 </sst>
 </file>
@@ -348,7 +375,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -358,6 +385,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -673,10 +703,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{532DE2F4-3B53-4E4D-BD5B-957BBCC0A7C1}">
-  <dimension ref="A1:C15"/>
+  <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -843,13 +873,46 @@
     </row>
     <row r="15" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B15" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="C15" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="C15" s="1" t="s">
+    </row>
+    <row r="16" spans="1:3" ht="72" x14ac:dyDescent="0.3">
+      <c r="A16" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C16" s="4" t="s">
         <v>44</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="72" x14ac:dyDescent="0.3">
+      <c r="A17" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="72" x14ac:dyDescent="0.3">
+      <c r="A18" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>51</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
new chloride data from IC run 3-3
</commit_message>
<xml_diff>
--- a/Data/Data_Citations.xlsx
+++ b/Data/Data_Citations.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\linne\Box Sync\CL_BUD\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B181170C-FFED-4B15-8C1F-ED4BAB4A7978}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D824A5CE-526E-4D96-94A7-869119F495F1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{02D620E8-8DA4-42D6-925F-9D866E7AA299}"/>
   </bookViews>
@@ -420,12 +420,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -440,7 +446,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -451,7 +457,13 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -770,8 +782,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{532DE2F4-3B53-4E4D-BD5B-957BBCC0A7C1}">
   <dimension ref="A1:C20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="G23" sqref="G23"/>
+    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -805,13 +817,13 @@
       </c>
     </row>
     <row r="3" spans="1:3" ht="55.2" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="5" t="s">
         <v>25</v>
       </c>
     </row>
@@ -838,35 +850,35 @@
       </c>
     </row>
     <row r="6" spans="1:3" ht="55.2" x14ac:dyDescent="0.3">
-      <c r="A6" s="1" t="s">
+      <c r="A6" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C6" s="5" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="187.2" x14ac:dyDescent="0.3">
-      <c r="A7" s="1" t="s">
+      <c r="A7" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="C7" s="4" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="144" x14ac:dyDescent="0.3">
-      <c r="A8" s="1" t="s">
+      <c r="A8" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B8" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="C8" s="4" t="s">
         <v>22</v>
       </c>
     </row>
@@ -926,13 +938,13 @@
       </c>
     </row>
     <row r="14" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A14" s="1" t="s">
+      <c r="A14" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="B14" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="C14" s="4" t="s">
         <v>37</v>
       </c>
     </row>
@@ -948,35 +960,35 @@
       </c>
     </row>
     <row r="16" spans="1:3" ht="72" x14ac:dyDescent="0.3">
-      <c r="A16" s="1" t="s">
+      <c r="A16" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="B16" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="C16" s="4" t="s">
+      <c r="C16" s="6" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="72" x14ac:dyDescent="0.3">
-      <c r="A17" s="1" t="s">
+      <c r="A17" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="B17" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="C17" s="4" t="s">
+      <c r="C17" s="6" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="72" x14ac:dyDescent="0.3">
-      <c r="A18" s="1" t="s">
+      <c r="A18" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="B18" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="C18" s="4" t="s">
+      <c r="C18" s="6" t="s">
         <v>51</v>
       </c>
     </row>

</xml_diff>